<commit_message>
20210718 add data to salary_type_mapping in hr_bank_code_mapping
</commit_message>
<xml_diff>
--- a/table_schema.xlsx
+++ b/table_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yichen/Desktop/hr_bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF10EA4-5850-A94E-A448-4C676C5A7D0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA7022-F1E7-844A-9CA8-E13EFA318941}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="460" windowWidth="28260" windowHeight="16780" xr2:uid="{E23C1A2C-3772-0A45-9F44-C5D6AB4FCA5D}"/>
   </bookViews>
@@ -2467,8 +2467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BF751F-C90B-5A40-8EEB-93D01660E6BD}">
   <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="114" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
20220207 add column definition
</commit_message>
<xml_diff>
--- a/table_schema.xlsx
+++ b/table_schema.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yichen/Desktop/hr_bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81F2C7B-C818-524D-B54B-99BD3E25440E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4288193-67B3-2D4B-ADD3-6F3143F83705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="460" windowWidth="28260" windowHeight="16780" xr2:uid="{E23C1A2C-3772-0A45-9F44-C5D6AB4FCA5D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ERD_v1" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
+    <sheet name="欄位中英參考" sheetId="3" r:id="rId1"/>
+    <sheet name="ERD_TEMP1" sheetId="1" r:id="rId2"/>
+    <sheet name="ERD_TEMP2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="387">
   <si>
     <t>job_id</t>
   </si>
@@ -1978,13 +1979,204 @@
   <si>
     <t>job_id</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文欄位</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文名稱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>例如：富邦人壽、北富銀，皆為「富邦」</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>定義不確定</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作類型</t>
+  </si>
+  <si>
+    <t>職缺說明</t>
+  </si>
+  <si>
+    <t>工作地區</t>
+  </si>
+  <si>
+    <t>性別json</t>
+  </si>
+  <si>
+    <t>學歷json</t>
+  </si>
+  <si>
+    <t>年齡json</t>
+  </si>
+  <si>
+    <t>工作經驗json</t>
+  </si>
+  <si>
+    <t>語言json</t>
+  </si>
+  <si>
+    <t>科系json</t>
+  </si>
+  <si>
+    <t>公司地區</t>
+  </si>
+  <si>
+    <t>薪水</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t># If salary_max is larger than salary_min by 25%, then set 125% of salary_min as salary_max.
+    if salary_max / salary_min &gt; 1.25:
+        salary_max = salary_min * 1.25</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求人數描述 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>男性應徵人數</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>女性應徵人數</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>國中小學歷應徵人數</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>高中學歷應徵人數</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>碩博士學歷應徵人數</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="PMingLiU"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>大學學歷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>應徵人數</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>20歲以下應徵人數</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文要求</t>
+  </si>
+  <si>
+    <t>日文要求</t>
+  </si>
+  <si>
+    <t>韓文要求</t>
+  </si>
+  <si>
+    <t>21~25歲應徵人數</t>
+  </si>
+  <si>
+    <t>26~30歲應徵人數</t>
+  </si>
+  <si>
+    <t>31~35歲應徵人數</t>
+  </si>
+  <si>
+    <t>36~40歲應徵人數</t>
+  </si>
+  <si>
+    <t>41~45歲應徵人數</t>
+  </si>
+  <si>
+    <t>46~50歲應徵人數</t>
+  </si>
+  <si>
+    <t>51~55歲應徵人數</t>
+  </si>
+  <si>
+    <t>56~60歲應徵人數</t>
+  </si>
+  <si>
+    <t>60歲以上應徵人數</t>
+  </si>
+  <si>
+    <t>無工作經驗應徵人數</t>
+  </si>
+  <si>
+    <t>1年以下經驗應徵人數</t>
+  </si>
+  <si>
+    <t>1~3年經驗應徵人數</t>
+  </si>
+  <si>
+    <t>3~5年經驗應徵人數</t>
+  </si>
+  <si>
+    <t>5~10年經驗應徵人數</t>
+  </si>
+  <si>
+    <t>10~15年經驗應徵人數</t>
+  </si>
+  <si>
+    <t>15~20年經驗應徵人數</t>
+  </si>
+  <si>
+    <t>20~25年經驗應徵人數</t>
+  </si>
+  <si>
+    <t>25年以上經驗應徵人數</t>
+  </si>
+  <si>
+    <t>資管系應徵人數</t>
+  </si>
+  <si>
+    <t>資工系應徵人數</t>
+  </si>
+  <si>
+    <t>統計系應徵人數</t>
+  </si>
+  <si>
+    <t>數理統計系應徵人數</t>
+  </si>
+  <si>
+    <t>Java專長應徵人數</t>
+  </si>
+  <si>
+    <t>Python專長應徵人數</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2078,8 +2270,24 @@
       <family val="1"/>
       <charset val="136"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2098,13 +2306,28 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -2113,7 +2336,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2157,6 +2380,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2472,11 +2704,938 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE3A68A-346C-2043-B244-396510BB2748}">
+  <dimension ref="A1:C111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16">
+      <c r="A1" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16">
+      <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16">
+      <c r="A14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16">
+      <c r="A16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16">
+      <c r="A17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16">
+      <c r="A18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16">
+      <c r="A19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16">
+      <c r="A20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16">
+      <c r="A21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16">
+      <c r="A22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C22" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16">
+      <c r="A23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16">
+      <c r="A24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16">
+      <c r="A25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16">
+      <c r="A26" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16">
+      <c r="A27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16">
+      <c r="A28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16">
+      <c r="A29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16">
+      <c r="A30" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="16">
+      <c r="A31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="16">
+      <c r="A32" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16">
+      <c r="A33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16">
+      <c r="A34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16">
+      <c r="A35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16">
+      <c r="A36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16">
+      <c r="A37" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16">
+      <c r="A38" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16">
+      <c r="A39" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16">
+      <c r="A40" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16">
+      <c r="A41" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16">
+      <c r="A42" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16">
+      <c r="A43" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16">
+      <c r="A44" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16">
+      <c r="A45" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16">
+      <c r="A46" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16">
+      <c r="A47" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16">
+      <c r="A48" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="16">
+      <c r="A49" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16">
+      <c r="A50" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16">
+      <c r="A51" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16">
+      <c r="A52" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16">
+      <c r="A53" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16">
+      <c r="A54" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16">
+      <c r="A55" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16">
+      <c r="A56" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16">
+      <c r="A57" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="16">
+      <c r="A58" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16">
+      <c r="A59" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16">
+      <c r="A60" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="16">
+      <c r="A61" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="16">
+      <c r="A62" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="16">
+      <c r="A63" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="16">
+      <c r="A64" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="16">
+      <c r="A65" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="16">
+      <c r="A66" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="16">
+      <c r="A67" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="16">
+      <c r="A68" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="16">
+      <c r="A69" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="16">
+      <c r="A70" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="16">
+      <c r="A71" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="16">
+      <c r="A72" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="16">
+      <c r="A73" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="16">
+      <c r="A74" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="16">
+      <c r="A75" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="64">
+      <c r="A76" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="16">
+      <c r="A77" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="16">
+      <c r="A78" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="16">
+      <c r="A79" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="16">
+      <c r="A80" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="16">
+      <c r="A81" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16">
+      <c r="A82" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="16">
+      <c r="A83" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="16">
+      <c r="A84" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="16">
+      <c r="A85" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B85" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="16">
+      <c r="A86" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B86" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="16">
+      <c r="A87" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="16">
+      <c r="A88" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="16">
+      <c r="A89" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B89" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="16">
+      <c r="A90" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B90" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="16">
+      <c r="A91" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="16">
+      <c r="A92" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B92" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="16">
+      <c r="A93" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B93" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16">
+      <c r="A94" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B94" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16">
+      <c r="A95" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B95" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16">
+      <c r="A96" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B96" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16">
+      <c r="A97" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B97" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16">
+      <c r="A98" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B98" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16">
+      <c r="A99" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B99" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16">
+      <c r="A100" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B100" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16">
+      <c r="A101" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B101" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="16">
+      <c r="A102" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B102" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16">
+      <c r="A103" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B103" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="16">
+      <c r="A104" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B104" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16">
+      <c r="A105" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B105" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16">
+      <c r="A106" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B106" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="16">
+      <c r="A107" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B107" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="16">
+      <c r="A108" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B108" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="16">
+      <c r="A109" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B109" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="16">
+      <c r="A110" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B110" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="16">
+      <c r="A111" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B111" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BF751F-C90B-5A40-8EEB-93D01660E6BD}">
   <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="114" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4355,11 +5514,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD3A391-4416-5E40-A82D-938567559D65}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="132" workbookViewId="0">
       <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>

</xml_diff>